<commit_message>
Add first player feedback
Change-Id: I6f64bfecd5ad16cf24e13c7707b4204cfe79ebe2
</commit_message>
<xml_diff>
--- a/Data/Game_Data.xlsx
+++ b/Data/Game_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12870" tabRatio="664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12870" tabRatio="664" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Food_Define" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="95">
   <si>
     <t>[Start]</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>ref:Game_Data:Response_ID</t>
-  </si>
-  <si>
-    <t>Stop Eating</t>
   </si>
   <si>
     <t>Name</t>
@@ -758,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,19 +801,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>6</v>
@@ -837,16 +834,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="12">
         <v>3</v>
@@ -860,16 +857,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="12">
         <v>3</v>
@@ -883,16 +880,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="12">
         <v>5</v>
@@ -906,16 +903,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="12">
         <v>5</v>
@@ -929,16 +926,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="12">
         <v>8</v>
@@ -952,16 +949,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="12">
         <v>8</v>
@@ -975,16 +972,16 @@
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="15">
         <v>8</v>
@@ -998,16 +995,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="C14" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="12">
         <v>3</v>
@@ -1021,16 +1018,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>52</v>
-      </c>
       <c r="C15" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -1044,16 +1041,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="C16" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16">
         <v>5</v>
@@ -1067,16 +1064,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="C17" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -1181,7 +1178,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1208,10 +1205,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1230,10 +1227,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -1241,10 +1238,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="15">
         <v>10</v>
@@ -1252,10 +1249,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="15">
         <v>10</v>
@@ -1263,10 +1260,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="15">
         <v>10</v>
@@ -1274,10 +1271,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="15">
         <v>10</v>
@@ -1285,10 +1282,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="15">
         <v>10</v>
@@ -1327,7 +1324,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1335,7 +1332,7 @@
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1349,13 +1346,13 @@
     </row>
     <row r="5" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -1365,7 +1362,7 @@
     </row>
     <row r="16" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1374,7 +1371,7 @@
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1392,7 +1389,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -1403,7 +1400,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -1415,7 +1412,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -1427,7 +1424,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1489,7 +1486,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1498,7 +1495,7 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1513,25 +1510,25 @@
     </row>
     <row r="5" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -1547,13 +1544,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="15">
         <v>1</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" s="15">
         <v>120</v>
@@ -1570,13 +1567,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="15">
         <v>2</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="15">
         <v>120</v>
@@ -1593,13 +1590,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="15">
         <v>3</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="15">
         <v>120</v>
@@ -1616,13 +1613,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="15">
         <v>4</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="15">
         <v>120</v>
@@ -1646,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,7 +1677,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
@@ -1690,12 +1687,11 @@
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="str">
-        <f>SUBSTITUTE(B7," ", "_")</f>
-        <v>Stop_Eating</v>
+      <c r="A7" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1776,7 +1772,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,7 +1794,7 @@
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1814,7 +1810,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>5</v>
@@ -2016,7 +2012,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,7 +2025,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2037,7 +2033,7 @@
     </row>
     <row r="2" spans="1:4" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2050,18 +2046,18 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>27</v>
@@ -2070,46 +2066,46 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2120,7 +2116,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,7 +2127,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,7 +2138,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,7 +2149,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2164,7 +2160,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2175,7 +2171,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2186,7 +2182,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2197,7 +2193,7 @@
         <v>22</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2208,7 +2204,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2219,7 +2215,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2230,7 +2226,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2241,7 +2237,7 @@
         <v>24</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2252,7 +2248,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2263,7 +2259,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2274,7 +2270,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2285,7 +2281,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add feedback for food
Change-Id: I5fb7d5ab373a9814f32957f4403e4cdd950e9f28
</commit_message>
<xml_diff>
--- a/Data/Game_Data.xlsx
+++ b/Data/Game_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ubisoft.org\MTRStudio\Production\OWLIENT\Commun\Studio\Luc Meys\La Cantina\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Projects\Perso\LaCantina\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="97">
   <si>
     <t>[Start]</t>
   </si>
@@ -56,18 +56,9 @@
     <t>Avocado</t>
   </si>
   <si>
-    <t>Broccoli</t>
-  </si>
-  <si>
-    <t>Aubergine</t>
-  </si>
-  <si>
     <t>Corn</t>
   </si>
   <si>
-    <t>Hamburger</t>
-  </si>
-  <si>
     <t>Food_Define</t>
   </si>
   <si>
@@ -275,9 +266,6 @@
     <t>Junk</t>
   </si>
   <si>
-    <t>Pancakes</t>
-  </si>
-  <si>
     <t>Fruit</t>
   </si>
   <si>
@@ -314,7 +302,25 @@
     <t>Reward</t>
   </si>
   <si>
-    <t>French Fries</t>
+    <t>Brocoli</t>
+  </si>
+  <si>
+    <t>Eggplant</t>
+  </si>
+  <si>
+    <t>Fries</t>
+  </si>
+  <si>
+    <t>Burger</t>
+  </si>
+  <si>
+    <t>Pancake</t>
+  </si>
+  <si>
+    <t>Cry</t>
+  </si>
+  <si>
+    <t>Play</t>
   </si>
 </sst>
 </file>
@@ -756,7 +762,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="C24" sqref="C24:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +777,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -801,19 +807,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>6</v>
@@ -834,16 +840,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E7" s="12">
         <v>3</v>
@@ -857,16 +863,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E8" s="12">
         <v>3</v>
@@ -880,16 +886,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E9" s="12">
         <v>5</v>
@@ -903,16 +909,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E10" s="12">
         <v>5</v>
@@ -926,16 +932,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E11" s="12">
         <v>8</v>
@@ -949,16 +955,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E12" s="12">
         <v>8</v>
@@ -972,16 +978,16 @@
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E13" s="15">
         <v>8</v>
@@ -995,16 +1001,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E14" s="12">
         <v>3</v>
@@ -1018,16 +1024,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -1041,16 +1047,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E16">
         <v>5</v>
@@ -1064,16 +1070,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -1178,7 +1184,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1205,10 +1211,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1227,10 +1233,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -1238,10 +1244,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C8" s="15">
         <v>10</v>
@@ -1249,10 +1255,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C9" s="15">
         <v>10</v>
@@ -1260,10 +1266,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C10" s="15">
         <v>10</v>
@@ -1271,10 +1277,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C11" s="15">
         <v>10</v>
@@ -1282,10 +1288,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C12" s="15">
         <v>10</v>
@@ -1324,7 +1330,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1332,7 +1338,7 @@
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1346,13 +1352,13 @@
     </row>
     <row r="5" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -1362,7 +1368,7 @@
     </row>
     <row r="16" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1371,7 +1377,7 @@
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1389,7 +1395,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -1400,7 +1406,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -1412,7 +1418,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -1424,7 +1430,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1486,7 +1492,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1495,7 +1501,7 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1510,25 +1516,25 @@
     </row>
     <row r="5" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -1544,13 +1550,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B7" s="15">
         <v>1</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D7" s="15">
         <v>120</v>
@@ -1567,13 +1573,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B8" s="15">
         <v>2</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D8" s="15">
         <v>120</v>
@@ -1590,13 +1596,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B9" s="15">
         <v>3</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D9" s="15">
         <v>120</v>
@@ -1613,13 +1619,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" s="15">
         <v>4</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10" s="15">
         <v>120</v>
@@ -1644,7 +1650,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,13 +1663,13 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4"/>
     </row>
@@ -1674,10 +1680,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.3">
@@ -1688,46 +1694,42 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="str">
-        <f>SUBSTITUTE(B8," ", "_")</f>
-        <v>Vomit</v>
+      <c r="A8" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="str">
-        <f>SUBSTITUTE(B9," ", "_")</f>
-        <v>Fight</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="str">
-        <f>SUBSTITUTE(B10," ", "_")</f>
-        <v>Playing</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="str">
-        <f>SUBSTITUTE(B11," ", "_")</f>
-        <v>Crying</v>
-      </c>
       <c r="B11" s="15" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1786,7 +1788,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1794,7 +1796,7 @@
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1807,10 +1809,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>5</v>
@@ -1831,10 +1833,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="15">
         <v>5</v>
@@ -1845,10 +1847,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="15">
         <v>2</v>
@@ -1859,10 +1861,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="15">
         <v>2</v>
@@ -1873,10 +1875,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="15">
         <v>5</v>
@@ -2025,7 +2027,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2033,7 +2035,7 @@
     </row>
     <row r="2" spans="1:4" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2046,242 +2048,242 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>22</v>
-      </c>
       <c r="C18" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>23</v>
-      </c>
       <c r="C20" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>24</v>
-      </c>
       <c r="C24" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Set level timer to 90s
Change-Id: Ic9e58e036038fc5b80515d30e63d2345203844e2
</commit_message>
<xml_diff>
--- a/Data/Game_Data.xlsx
+++ b/Data/Game_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12870" tabRatio="664" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12870" tabRatio="664"/>
   </bookViews>
   <sheets>
     <sheet name="Food_Define" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="98">
   <si>
     <t>[Start]</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>Play</t>
+  </si>
+  <si>
+    <t>Waiting</t>
   </si>
 </sst>
 </file>
@@ -761,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +827,9 @@
       <c r="G5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="6" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
@@ -836,7 +841,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -860,6 +865,9 @@
       <c r="G7" s="13">
         <v>20</v>
       </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
@@ -883,6 +891,9 @@
       <c r="G8" s="13">
         <v>20</v>
       </c>
+      <c r="H8" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -906,6 +917,9 @@
       <c r="G9" s="13">
         <v>10</v>
       </c>
+      <c r="H9" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -929,6 +943,9 @@
       <c r="G10" s="13">
         <v>10</v>
       </c>
+      <c r="H10" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
@@ -952,6 +969,9 @@
       <c r="G11" s="13">
         <v>5</v>
       </c>
+      <c r="H11" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -975,6 +995,9 @@
       <c r="G12" s="13">
         <v>5</v>
       </c>
+      <c r="H12" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
@@ -998,6 +1021,9 @@
       <c r="G13" s="15">
         <v>5</v>
       </c>
+      <c r="H13" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
@@ -1021,6 +1047,9 @@
       <c r="G14" s="13">
         <v>20</v>
       </c>
+      <c r="H14" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
@@ -1044,6 +1073,9 @@
       <c r="G15">
         <v>20</v>
       </c>
+      <c r="H15" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
@@ -1067,8 +1099,11 @@
       <c r="G16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>51</v>
       </c>
@@ -1090,68 +1125,71 @@
       <c r="G17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -1477,7 +1515,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,7 +1597,7 @@
         <v>63</v>
       </c>
       <c r="D7" s="15">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="E7" s="15">
         <v>3</v>
@@ -1582,7 +1620,7 @@
         <v>63</v>
       </c>
       <c r="D8" s="15">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="E8" s="15">
         <v>4</v>
@@ -1605,7 +1643,7 @@
         <v>63</v>
       </c>
       <c r="D9" s="15">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="E9" s="15">
         <v>5</v>
@@ -1628,7 +1666,7 @@
         <v>63</v>
       </c>
       <c r="D10" s="15">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="E10" s="15">
         <v>6</v>
@@ -1649,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update inputs and timer
Change-Id: I93bed732e11442d1c541675816733dbf428ac269
</commit_message>
<xml_diff>
--- a/Data/Game_Data.xlsx
+++ b/Data/Game_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12870" tabRatio="664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12870" tabRatio="664" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Food_Define" sheetId="1" r:id="rId1"/>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1597,7 @@
         <v>63</v>
       </c>
       <c r="D7" s="15">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E7" s="15">
         <v>3</v>
@@ -1620,7 +1620,7 @@
         <v>63</v>
       </c>
       <c r="D8" s="15">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E8" s="15">
         <v>4</v>
@@ -1643,7 +1643,7 @@
         <v>63</v>
       </c>
       <c r="D9" s="15">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E9" s="15">
         <v>5</v>
@@ -1666,7 +1666,7 @@
         <v>63</v>
       </c>
       <c r="D10" s="15">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E10" s="15">
         <v>6</v>
@@ -1812,7 +1812,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="A9" sqref="A9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,7 +2052,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>